<commit_message>
Initial experiment data collection complete.
</commit_message>
<xml_diff>
--- a/ResultsForTrialSetOne.xlsx
+++ b/ResultsForTrialSetOne.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Nextcloud\PersonalProjects\selective_order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF3C639-1261-43C5-8B7D-8EDB16B7FFAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522112DE-8CDC-4A35-A181-5C55F422A42B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="3300" windowWidth="21825" windowHeight="14235" xr2:uid="{61419BD0-A300-4EE3-B60B-1256866A2BCD}"/>
+    <workbookView xWindow="21285" yWindow="5820" windowWidth="21825" windowHeight="14235" xr2:uid="{61419BD0-A300-4EE3-B60B-1256866A2BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Loss</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Total Epochs</t>
+  </si>
+  <si>
+    <t>4 Epochs Standard Learner</t>
+  </si>
+  <si>
+    <t>1 Epoch Adversary FGSM, 3 Epoch Standard Learner (Weight Copy)</t>
+  </si>
+  <si>
+    <t>5 Epochs Standard Learner</t>
+  </si>
+  <si>
+    <t>MNIST Dataset Experiment</t>
   </si>
 </sst>
 </file>
@@ -113,6 +125,1359 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MNIST</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Dataset Selective Injection Experiment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1 Epoch Adversary FGSM, 1 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Epoch Adversary FGSM, 2 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Epoch Adversary FGSM, 3 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Epcoch Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5 Epochs Standard Learner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.9623999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2914000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3936000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8478000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0647</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8ED4-4A47-9B31-EFD3D7097862}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1 Epoch Adversary FGSM, 1 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Epoch Adversary FGSM, 2 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Epoch Adversary FGSM, 3 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Epcoch Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5 Epochs Standard Learner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.35420000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79169999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64580000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.80210000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8ED4-4A47-9B31-EFD3D7097862}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1 Epoch Adversary FGSM, 1 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Epoch Adversary FGSM, 2 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Epoch Adversary FGSM, 3 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Epcoch Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5 Epochs Standard Learner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.9715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2033999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9995000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7817000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.736</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8ED4-4A47-9B31-EFD3D7097862}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1 Epoch Adversary FGSM, 1 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Epoch Adversary FGSM, 2 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Epoch Adversary FGSM, 3 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Epcoch Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5 Epochs Standard Learner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.42570000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51149999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53990000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35820000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44340000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44969999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55700000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8ED4-4A47-9B31-EFD3D7097862}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Epochs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1 Epoch Adversary FGSM, 1 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Epoch Adversary FGSM, 2 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1 Epoch Adversary FGSM, 3 Epoch Standard Learner (Weight Copy)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Epcoch Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4 Epochs Standard Learner</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5 Epochs Standard Learner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8ED4-4A47-9B31-EFD3D7097862}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="75176704"/>
+        <c:axId val="75042272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75176704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75042272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75042272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75176704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0701402-31B7-4DED-B9D4-FB04EF76A8C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C142B9F5-AFB3-403F-958D-A00CF9285D8C}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0">
+  <autoFilter ref="A1:F9" xr:uid="{D7D5DC75-915E-47C8-BD67-251D24DFCD2F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{20B0605F-486F-4860-8D46-BC33082F39BF}" name="MNIST Dataset Experiment"/>
+    <tableColumn id="2" xr3:uid="{AA7331A0-7C1F-44DB-BAF6-52A14A5F43D7}" name="Loss"/>
+    <tableColumn id="3" xr3:uid="{8C068375-AE56-40C0-854C-AB753ACE16B1}" name="Accuracy"/>
+    <tableColumn id="4" xr3:uid="{87DB76D2-9C36-445B-B12F-CBA195164440}" name="Validation Loss"/>
+    <tableColumn id="5" xr3:uid="{A2285133-D17E-4AFD-B6C4-1FDF0AB7756A}" name="Validation Accuracy"/>
+    <tableColumn id="6" xr3:uid="{3E351232-FB68-404B-B28C-1AF1BA2FD0E1}" name="Total Epochs"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B85FAE1-64BE-446F-A77A-1272770813D0}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,11 +1788,14 @@
     <col min="1" max="1" width="69.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -486,65 +1854,129 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1.2914000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.79169999999999996</v>
+      </c>
+      <c r="D4">
+        <v>1.6012</v>
+      </c>
+      <c r="E4">
+        <v>0.53990000000000005</v>
+      </c>
+      <c r="F4">
         <v>4</v>
-      </c>
-      <c r="B4">
-        <v>2.3936000000000002</v>
-      </c>
-      <c r="C4">
-        <v>0.13539999999999999</v>
-      </c>
-      <c r="D4">
-        <v>2.2033999999999998</v>
-      </c>
-      <c r="E4">
-        <v>0.20749999999999999</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>1.8478000000000001</v>
+        <v>2.3936000000000002</v>
       </c>
       <c r="C5">
-        <v>0.4375</v>
+        <v>0.13539999999999999</v>
       </c>
       <c r="D5">
-        <v>1.9995000000000001</v>
+        <v>2.2033999999999998</v>
       </c>
       <c r="E5">
-        <v>0.35820000000000002</v>
+        <v>0.20749999999999999</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1.8478000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.4375</v>
+      </c>
+      <c r="D6">
+        <v>1.9995000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.35820000000000002</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1.5944</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>0.64580000000000004</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>1.7817000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>0.44340000000000002</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>1.3105</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>1.736</v>
+      </c>
+      <c r="E8">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1.0647</v>
+      </c>
+      <c r="C9">
+        <v>0.80210000000000004</v>
+      </c>
+      <c r="D9">
+        <v>1.5467</v>
+      </c>
+      <c r="E9">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new dataset experiment.
</commit_message>
<xml_diff>
--- a/ResultsForTrialSetOne.xlsx
+++ b/ResultsForTrialSetOne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Nextcloud\PersonalProjects\selective_order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522112DE-8CDC-4A35-A181-5C55F422A42B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430E1FF5-1D05-4474-91BD-65F3F11A8D75}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21285" yWindow="5820" windowWidth="21825" windowHeight="14235" xr2:uid="{61419BD0-A300-4EE3-B60B-1256866A2BCD}"/>
+    <workbookView xWindow="16290" yWindow="6900" windowWidth="21825" windowHeight="14235" xr2:uid="{61419BD0-A300-4EE3-B60B-1256866A2BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Dataset Selective Injection Experiment</a:t>
+              <a:t> Selective Injection Experiment</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>

</xml_diff>

<commit_message>
Added build model function.
</commit_message>
<xml_diff>
--- a/ResultsForTrialSetOne.xlsx
+++ b/ResultsForTrialSetOne.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Nextcloud\PersonalProjects\selective_order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430E1FF5-1D05-4474-91BD-65F3F11A8D75}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AC74B1-A251-4B29-AD48-7EAE4546836B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16290" yWindow="6900" windowWidth="21825" windowHeight="14235" xr2:uid="{61419BD0-A300-4EE3-B60B-1256866A2BCD}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     <t>5 Epochs Standard Learner</t>
   </si>
   <si>
-    <t>MNIST Dataset Experiment</t>
+    <t>MNIST Dataset Experiment (96 Samples)</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1469,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C142B9F5-AFB3-403F-958D-A00CF9285D8C}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0">
   <autoFilter ref="A1:F9" xr:uid="{D7D5DC75-915E-47C8-BD67-251D24DFCD2F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{20B0605F-486F-4860-8D46-BC33082F39BF}" name="MNIST Dataset Experiment"/>
+    <tableColumn id="1" xr3:uid="{20B0605F-486F-4860-8D46-BC33082F39BF}" name="MNIST Dataset Experiment (96 Samples)"/>
     <tableColumn id="2" xr3:uid="{AA7331A0-7C1F-44DB-BAF6-52A14A5F43D7}" name="Loss"/>
     <tableColumn id="3" xr3:uid="{8C068375-AE56-40C0-854C-AB753ACE16B1}" name="Accuracy"/>
     <tableColumn id="4" xr3:uid="{87DB76D2-9C36-445B-B12F-CBA195164440}" name="Validation Loss"/>
@@ -1779,9 +1779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B85FAE1-64BE-446F-A77A-1272770813D0}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>